<commit_message>
refactor: update SQL query parameters, add nodemon dependency, and improve error handling
</commit_message>
<xml_diff>
--- a/files/template/Randy-Hariadi-2022-12.xlsx
+++ b/files/template/Randy-Hariadi-2022-12.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>DAFTAR HASIL PLAGIAT (TURNITIN) MAHASISWA</t>
   </si>
@@ -151,9 +151,6 @@
     <t>undefined-12</t>
   </si>
   <si>
-    <t>Lis Indriani</t>
-  </si>
-  <si>
     <t>Hasrullah dg naba</t>
   </si>
   <si>
@@ -163,9 +160,6 @@
     <t>mirfayana mirfa</t>
   </si>
   <si>
-    <t>10584101818</t>
-  </si>
-  <si>
     <t>1059411101010</t>
   </si>
   <si>
@@ -175,9 +169,6 @@
     <t>105190043571</t>
   </si>
   <si>
-    <t>Pentingnya Hubungan Internasional dalam hubungan diploma sehingga iya</t>
-  </si>
-  <si>
     <t>Proses penciptaan budha dalam keagamaan hindu serta bagaimana kelanjutan hidup krisna</t>
   </si>
   <si>
@@ -187,33 +178,24 @@
     <t>analisis tingkat kepuasan pemustaka</t>
   </si>
   <si>
+    <t>Profesi Dokter</t>
+  </si>
+  <si>
+    <t>Pendidikan Bahasa Arab</t>
+  </si>
+  <si>
     <t>Pendidikan Agama Islam</t>
   </si>
   <si>
-    <t>Profesi Dokter</t>
-  </si>
-  <si>
-    <t>Pendidikan Bahasa Arab</t>
-  </si>
-  <si>
-    <t>91%</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
-    <t>11%</t>
+    <t>100000</t>
   </si>
   <si>
     <t>50000</t>
   </si>
   <si>
-    <t>100000</t>
-  </si>
-  <si>
-    <t>07-12-2022</t>
-  </si>
-  <si>
     <t>15-12-2022</t>
   </si>
   <si>
@@ -221,9 +203,6 @@
   </si>
   <si>
     <t>17-12-2022</t>
-  </si>
-  <si>
-    <t>Bank Rakyat Indonesia</t>
   </si>
   <si>
     <t>Bank Merakyat</t>
@@ -1532,8 +1511,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" dataDxfId="26" displayName="Table2" headerRowDxfId="27" id="2" mc:Ignorable="xr xr3" name="Table2" ref="E4:E9" tableBorderDxfId="25" totalsRowShown="0" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}">
-  <autoFilter ref="E4:E9" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" dataDxfId="26" displayName="Table2" headerRowDxfId="27" id="2" mc:Ignorable="xr xr3" name="Table2" ref="E4:E8" tableBorderDxfId="25" totalsRowShown="0" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}">
+  <autoFilter ref="E4:E8" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="1">
     <tableColumn dataDxfId="24" id="1" name="JURUSAN" xr3:uid="{00000000-0010-0000-0100-000001000000}"/>
   </tableColumns>
@@ -1542,8 +1521,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" dataDxfId="21" displayName="Table4" headerRowBorderDxfId="22" headerRowDxfId="23" id="4" mc:Ignorable="xr xr3" name="Table4" ref="F5:K9" tableBorderDxfId="20" totalsRowShown="0" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}">
-  <autoFilter ref="F5:K9" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" dataDxfId="21" displayName="Table4" headerRowBorderDxfId="22" headerRowDxfId="23" id="4" mc:Ignorable="xr xr3" name="Table4" ref="F5:K8" tableBorderDxfId="20" totalsRowShown="0" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}">
+  <autoFilter ref="F5:K8" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="6">
     <tableColumn dataDxfId="19" id="1" name="PROPOSAL" xr3:uid="{00000000-0010-0000-0200-000001000000}"/>
     <tableColumn dataDxfId="18" id="2" name="HASIL" xr3:uid="{00000000-0010-0000-0200-000002000000}"/>
@@ -1567,8 +1546,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" dataDxfId="7" displayName="Table6" headerRowBorderDxfId="8" headerRowDxfId="9" id="6" mc:Ignorable="xr xr3" name="Table6" ref="M4:M9" tableBorderDxfId="6" totalsRowBorderDxfId="5" totalsRowShown="0" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}">
-  <autoFilter ref="M4:M9" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" dataDxfId="7" displayName="Table6" headerRowBorderDxfId="8" headerRowDxfId="9" id="6" mc:Ignorable="xr xr3" name="Table6" ref="M4:M8" tableBorderDxfId="6" totalsRowBorderDxfId="5" totalsRowShown="0" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}">
+  <autoFilter ref="M4:M8" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="1">
     <tableColumn dataDxfId="4" id="1" name="TANGGAL PEMBAYARAN" xr3:uid="{00000000-0010-0000-0400-000001000000}"/>
   </tableColumns>
@@ -1577,8 +1556,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" dataDxfId="2" displayName="Table7" headerRowDxfId="3" id="7" mc:Ignorable="xr xr3" name="Table7" ref="N4:N9" tableBorderDxfId="1" totalsRowShown="0" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}">
-  <autoFilter ref="N4:N9" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" dataDxfId="2" displayName="Table7" headerRowDxfId="3" id="7" mc:Ignorable="xr xr3" name="Table7" ref="N4:N8" tableBorderDxfId="1" totalsRowShown="0" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}">
+  <autoFilter ref="N4:N8" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="1">
     <tableColumn dataDxfId="0" id="1" name="BANK" xr3:uid="{00000000-0010-0000-0500-000001000000}"/>
   </tableColumns>
@@ -1849,7 +1828,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" zoomScale="92" zoomScaleNormal="145">
       <selection activeCell="G12" sqref="G12"/>
@@ -1994,158 +1973,128 @@
     </row>
     <row ht="27" r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="27">
-        <v>44</v>
+        <v>78</v>
       </c>
       <c r="B6" s="27" t="s">
         <v>43</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E6" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="F6" s="25" t="s">
-        <v>58</v>
-      </c>
       <c r="G6" s="25" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H6" s="25" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="I6" s="25"/>
       <c r="J6" s="25"/>
       <c r="K6" s="26" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="L6" s="27"/>
       <c r="M6" s="30" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="N6" s="31" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row ht="27" r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="27">
-        <v>78</v>
+        <v>123</v>
       </c>
       <c r="B7" s="27" t="s">
         <v>44</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F7" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="K7" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="M7" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="G7" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="H7" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="K7" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="M7" s="30" t="s">
-        <v>64</v>
-      </c>
       <c r="N7" s="31" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row ht="27" r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="27">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B8" s="27" t="s">
         <v>45</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E8" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="K8" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="F8" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="G8" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="H8" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="K8" s="26" t="s">
-        <v>61</v>
-      </c>
       <c r="M8" s="30" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="N8" s="31" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
-    <row ht="27" r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="27">
-        <v>125</v>
-      </c>
-      <c r="B9" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="E9" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="F9" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="G9" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="H9" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="K9" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="M9" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="N9" s="31" t="s">
-        <v>69</v>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32">
+        <v>200000</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="32">
-        <v>250000</v>
-      </c>
+      <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C11" s="2"/>
@@ -2167,100 +2116,95 @@
       <c r="D14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="K15" s="2"/>
+    <row ht="15" r="17" spans="1:14" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row customHeight="1" ht="18" r="18" spans="1:14" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="43"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="44"/>
     </row>
-    <row ht="15" r="18" spans="1:14" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row customHeight="1" ht="18" r="19" spans="1:14" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="42" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="43"/>
-      <c r="C19" s="43"/>
-      <c r="D19" s="43"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="44"/>
+    <row customHeight="1" ht="18" r="19" spans="1:12" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="46"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="46"/>
+      <c r="E19" s="46"/>
+      <c r="F19" s="47"/>
     </row>
-    <row customHeight="1" ht="18" r="20" spans="1:12" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="45" t="s">
-        <v>59</v>
-      </c>
-      <c r="B20" s="46"/>
-      <c r="C20" s="46"/>
-      <c r="D20" s="46"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="47"/>
+    <row ht="15" r="20" spans="1:12" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
     </row>
     <row ht="15" r="21" spans="1:12" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
+      <c r="A21" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="K21" s="2"/>
+      <c r="L21" s="6"/>
     </row>
-    <row ht="15" r="22" spans="1:12" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="9" t="s">
-        <v>18</v>
+    <row ht="16.2" r="22" spans="1:12" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="9">
+        <v>1</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="D22" s="41" t="s">
-        <v>20</v>
-      </c>
-      <c r="E22" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="G22" s="10" t="s">
-        <v>21</v>
+        <v>63</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F22" s="12">
+        <v>200000</v>
+      </c>
+      <c r="G22" s="13">
+        <v>200000</v>
       </c>
       <c r="K22" s="2"/>
       <c r="L22" s="6"/>
     </row>
-    <row ht="16.2" r="23" spans="1:12" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="9">
-        <v>1</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="F23" s="12">
-        <v>250000</v>
-      </c>
-      <c r="G23" s="13">
-        <v>250000</v>
-      </c>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="6"/>
       <c r="K23" s="2"/>
-      <c r="L23" s="6"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="6"/>
-      <c r="K24" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A18:F18"/>
     <mergeCell ref="A19:F19"/>
-    <mergeCell ref="A20:F20"/>
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="A2:M2"/>
     <mergeCell ref="A3:M3"/>

</xml_diff>